<commit_message>
Recalculated the leidingweerstand with new pt10 offsets
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Leidingweerstand/Leidingweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Leidingweerstand/Leidingweerstand_modelcoefficienten.xlsx
@@ -521,7 +521,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42705162046</v>
+        <v>45699.43251926496</v>
       </c>
     </row>
     <row r="3">
@@ -538,7 +538,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42705162046</v>
+        <v>45699.43251926496</v>
       </c>
     </row>
     <row r="4">
@@ -555,7 +555,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42705183385</v>
+        <v>45699.43251943853</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42705162046</v>
+        <v>45699.43251926496</v>
       </c>
     </row>
     <row r="6">
@@ -589,7 +589,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42705162046</v>
+        <v>45699.43251926496</v>
       </c>
     </row>
   </sheetData>
@@ -641,13 +641,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.238091056855733e-05</v>
+        <v>-1.221324539105585e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42494814815</v>
+        <v>45699.43113275463</v>
       </c>
     </row>
     <row r="3">
@@ -658,13 +658,13 @@
         <v>42319</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.396638056855733e-05</v>
+        <v>-1.379871539105585e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42494839121</v>
+        <v>45699.43113288195</v>
       </c>
     </row>
     <row r="4">
@@ -675,13 +675,13 @@
         <v>43057.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.487473556855733e-05</v>
+        <v>-1.470707039105585e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42494839121</v>
+        <v>45699.43113288195</v>
       </c>
     </row>
     <row r="5">
@@ -692,13 +692,13 @@
         <v>43355</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.524066056855733e-05</v>
+        <v>-1.507299539105585e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42494839121</v>
+        <v>45699.43113288195</v>
       </c>
     </row>
     <row r="6">
@@ -709,13 +709,13 @@
         <v>43418</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.291896438077007e-05</v>
+        <v>-1.266712723704561e-05</v>
       </c>
       <c r="D6" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42494814815</v>
+        <v>45699.43113275463</v>
       </c>
     </row>
     <row r="7">
@@ -726,13 +726,13 @@
         <v>43719</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.328919438077007e-05</v>
+        <v>-1.303735723704561e-05</v>
       </c>
       <c r="D7" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45693.42494839121</v>
+        <v>45699.43113288195</v>
       </c>
     </row>
     <row r="8">
@@ -743,13 +743,13 @@
         <v>44464.5</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.324982399105724e-05</v>
+        <v>-1.297767193405733e-05</v>
       </c>
       <c r="D8" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45693.42494814815</v>
+        <v>45699.43113275463</v>
       </c>
     </row>
     <row r="9">
@@ -760,13 +760,13 @@
         <v>45224</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.21257814130584e-05</v>
+        <v>-1.187982916669219e-05</v>
       </c>
       <c r="D9" t="n">
         <v>-1.23e-09</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>45693.42494814815</v>
+        <v>45699.43113275463</v>
       </c>
     </row>
   </sheetData>
@@ -818,13 +818,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.119204855739267e-06</v>
+        <v>-4.872309283647548e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-1.4e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42515686343</v>
+        <v>45699.43130829861</v>
       </c>
     </row>
     <row r="3">
@@ -835,13 +835,13 @@
         <v>42350.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-5.618142388860458e-06</v>
+        <v>-4.156400780547415e-06</v>
       </c>
       <c r="D3" t="n">
         <v>-1.4e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42515686343</v>
+        <v>45699.43130829861</v>
       </c>
     </row>
     <row r="4">
@@ -852,13 +852,13 @@
         <v>43428.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-7.127342388860458e-06</v>
+        <v>-5.665600780547415e-06</v>
       </c>
       <c r="D4" t="n">
         <v>-1.4e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42515716435</v>
+        <v>45699.43130847222</v>
       </c>
     </row>
     <row r="5">
@@ -869,13 +869,13 @@
         <v>43792.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-5.82783900820436e-06</v>
+        <v>-4.568058226027852e-06</v>
       </c>
       <c r="D5" t="n">
         <v>-1.4e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42515686343</v>
+        <v>45699.43130829861</v>
       </c>
     </row>
     <row r="6">
@@ -886,13 +886,13 @@
         <v>44807.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-5.23546054289103e-06</v>
+        <v>-3.896168531125502e-06</v>
       </c>
       <c r="D6" t="n">
         <v>-1.4e-09</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42515686343</v>
+        <v>45699.43130829861</v>
       </c>
     </row>
   </sheetData>
@@ -944,13 +944,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.017393637651924e-06</v>
+        <v>-8.116782944590257e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-1.37e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42539233797</v>
+        <v>45699.43149399306</v>
       </c>
     </row>
     <row r="3">
@@ -961,13 +961,13 @@
         <v>42049.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-7.414108637651924e-06</v>
+        <v>-9.513497944590258e-06</v>
       </c>
       <c r="D3" t="n">
         <v>-1.37e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.4253924537</v>
+        <v>45699.43149405093</v>
       </c>
     </row>
     <row r="4">
@@ -978,13 +978,13 @@
         <v>43446</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.327313637651924e-06</v>
+        <v>-1.142670294459026e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-1.37e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.4253924537</v>
+        <v>45699.43149405093</v>
       </c>
     </row>
     <row r="5">
@@ -995,13 +995,13 @@
         <v>43841.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-5.87125006710386e-06</v>
+        <v>-8.229782176666178e-06</v>
       </c>
       <c r="D5" t="n">
         <v>-1.37e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42539233797</v>
+        <v>45699.43149399306</v>
       </c>
     </row>
   </sheetData>
@@ -1053,13 +1053,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.433263747850981e-06</v>
+        <v>-8.259252009415245e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42553521991</v>
+        <v>45699.43161613426</v>
       </c>
     </row>
     <row r="3">
@@ -1070,13 +1070,13 @@
         <v>43068</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.025275467555059e-05</v>
+        <v>-1.141779515795446e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42553521991</v>
+        <v>45699.43161613426</v>
       </c>
     </row>
     <row r="4">
@@ -1087,13 +1087,13 @@
         <v>44104</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.194909794635769e-05</v>
+        <v>-1.336274291691822e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42553521991</v>
+        <v>45699.43161613426</v>
       </c>
     </row>
     <row r="5">
@@ -1104,13 +1104,13 @@
         <v>44895</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.012788190264657e-05</v>
+        <v>-1.123170811703284e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42553521991</v>
+        <v>45699.43161613426</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1168,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42563642361</v>
+        <v>45699.43168528935</v>
       </c>
     </row>
     <row r="3">
@@ -1185,7 +1185,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42563642361</v>
+        <v>45699.43168528935</v>
       </c>
     </row>
     <row r="4">
@@ -1202,7 +1202,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42563642361</v>
+        <v>45699.43168528935</v>
       </c>
     </row>
     <row r="5">
@@ -1219,7 +1219,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42563642361</v>
+        <v>45699.43168528935</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1277,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42575445602</v>
+        <v>45699.43174952547</v>
       </c>
     </row>
     <row r="3">
@@ -1294,7 +1294,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42575445602</v>
+        <v>45699.43174952547</v>
       </c>
     </row>
     <row r="4">
@@ -1311,7 +1311,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42575445602</v>
+        <v>45699.43174952547</v>
       </c>
     </row>
     <row r="5">
@@ -1328,7 +1328,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42575445602</v>
+        <v>45699.43174952547</v>
       </c>
     </row>
   </sheetData>
@@ -1380,13 +1380,13 @@
         <v>42371</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.954850676268416e-06</v>
+        <v>-4.618037803610032e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-2.5e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42586417824</v>
+        <v>45699.43181354167</v>
       </c>
     </row>
     <row r="3">
@@ -1397,13 +1397,13 @@
         <v>43533.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.124221653567186e-05</v>
+        <v>-3.295375806206255e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-2.5e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42586417824</v>
+        <v>45699.43181354167</v>
       </c>
     </row>
     <row r="4">
@@ -1414,13 +1414,13 @@
         <v>43897.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-7.359759328966005e-06</v>
+        <v>-8.884070366833857e-06</v>
       </c>
       <c r="D4" t="n">
         <v>-2.5e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42586417824</v>
+        <v>45699.43181354167</v>
       </c>
     </row>
     <row r="5">
@@ -1431,13 +1431,13 @@
         <v>44569.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.543541496129445e-06</v>
+        <v>-9.004647745344225e-06</v>
       </c>
       <c r="D5" t="n">
         <v>-2.5e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42586417824</v>
+        <v>45699.43181354167</v>
       </c>
     </row>
     <row r="6">
@@ -1448,13 +1448,13 @@
         <v>44912.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.155182937712057e-06</v>
+        <v>-8.861420220038791e-06</v>
       </c>
       <c r="D6" t="n">
         <v>-2.5e-08</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42586417824</v>
+        <v>45699.43181354167</v>
       </c>
     </row>
   </sheetData>
@@ -1512,7 +1512,7 @@
         <v>-2.8e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42595226852</v>
+        <v>45699.43187165509</v>
       </c>
     </row>
     <row r="3">
@@ -1529,7 +1529,7 @@
         <v>-2.8e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42595226852</v>
+        <v>45699.43187165509</v>
       </c>
     </row>
     <row r="4">
@@ -1546,7 +1546,7 @@
         <v>-2.8e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42595226852</v>
+        <v>45699.43187165509</v>
       </c>
     </row>
     <row r="5">
@@ -1563,7 +1563,7 @@
         <v>-2.8e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42595226852</v>
+        <v>45699.43187165509</v>
       </c>
     </row>
   </sheetData>
@@ -1615,13 +1615,13 @@
         <v>42371</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.627232742458986e-05</v>
+        <v>-1.073793294475766e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-1.4e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42605063658</v>
+        <v>45699.43192857639</v>
       </c>
     </row>
     <row r="3">
@@ -1632,13 +1632,13 @@
         <v>42812.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-2.114898546343843e-05</v>
+        <v>-8.874197228997538e-06</v>
       </c>
       <c r="D3" t="n">
         <v>-1.4e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42605063658</v>
+        <v>45699.43192857639</v>
       </c>
     </row>
     <row r="4">
@@ -1649,13 +1649,13 @@
         <v>43477.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.684665080964601e-05</v>
+        <v>-1.358832151727803e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-1.4e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42605063658</v>
+        <v>45699.43192857639</v>
       </c>
     </row>
     <row r="5">
@@ -1666,13 +1666,13 @@
         <v>43803</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.325631617934293e-05</v>
+        <v>-5.911167995260177e-06</v>
       </c>
       <c r="D5" t="n">
         <v>-1.4e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42605063658</v>
+        <v>45699.43192857639</v>
       </c>
     </row>
     <row r="6">
@@ -1683,13 +1683,13 @@
         <v>45325.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.673846913200857e-05</v>
+        <v>-2.473713047701173e-10</v>
       </c>
       <c r="D6" t="n">
         <v>-1.4e-08</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42605063658</v>
+        <v>45699.43192857639</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1747,7 @@
         <v>-1e-07</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42614628472</v>
+        <v>45699.43198909723</v>
       </c>
     </row>
     <row r="3">
@@ -1764,7 +1764,7 @@
         <v>-1e-07</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42614628472</v>
+        <v>45699.43198909723</v>
       </c>
     </row>
     <row r="4">
@@ -1781,7 +1781,7 @@
         <v>-1e-07</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42614628472</v>
+        <v>45699.43198909723</v>
       </c>
     </row>
   </sheetData>
@@ -1833,13 +1833,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-9.82656184701856e-06</v>
+        <v>-8.653514780392828e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-1.2e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42192086806</v>
+        <v>45699.42913420139</v>
       </c>
     </row>
     <row r="3">
@@ -1850,13 +1850,13 @@
         <v>43015.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.220916184701856e-05</v>
+        <v>-1.103611478039283e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-1.2e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42192101852</v>
+        <v>45699.42913428241</v>
       </c>
     </row>
     <row r="4">
@@ -1867,13 +1867,13 @@
         <v>43390</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.247325162580846e-05</v>
+        <v>-1.084727434972205e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-1.2e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42192086806</v>
+        <v>45699.42913420139</v>
       </c>
     </row>
     <row r="5">
@@ -1884,13 +1884,13 @@
         <v>44443.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.147833470576881e-05</v>
+        <v>-9.957755712075037e-06</v>
       </c>
       <c r="D5" t="n">
         <v>-1.2e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42192086806</v>
+        <v>45699.42913420139</v>
       </c>
     </row>
   </sheetData>
@@ -1948,7 +1948,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42624354167</v>
+        <v>45699.43204844907</v>
       </c>
     </row>
     <row r="3">
@@ -1965,7 +1965,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42624354167</v>
+        <v>45699.43204844907</v>
       </c>
     </row>
     <row r="4">
@@ -1982,7 +1982,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42624354167</v>
+        <v>45699.43204844907</v>
       </c>
     </row>
     <row r="5">
@@ -1999,7 +1999,7 @@
         <v>-1.8e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42624354167</v>
+        <v>45699.43204844907</v>
       </c>
     </row>
   </sheetData>
@@ -2057,7 +2057,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42637120371</v>
+        <v>45699.43212153935</v>
       </c>
     </row>
     <row r="3">
@@ -2074,7 +2074,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42637120371</v>
+        <v>45699.43212153935</v>
       </c>
     </row>
     <row r="4">
@@ -2091,7 +2091,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42637120371</v>
+        <v>45699.43212153935</v>
       </c>
     </row>
     <row r="5">
@@ -2108,7 +2108,7 @@
         <v>-2e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42637120371</v>
+        <v>45699.43212153935</v>
       </c>
     </row>
   </sheetData>
@@ -2160,13 +2160,13 @@
         <v>42370</v>
       </c>
       <c r="C2" t="n">
-        <v>-4.498825050988893e-05</v>
+        <v>-5.912817899241044e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42662696759</v>
+        <v>45699.43227958334</v>
       </c>
     </row>
     <row r="3">
@@ -2177,13 +2177,13 @@
         <v>43141.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.884575050988893e-05</v>
+        <v>-6.298567899241044e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42662719907</v>
+        <v>45699.43227981481</v>
       </c>
     </row>
     <row r="4">
@@ -2194,13 +2194,13 @@
         <v>43509</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.393411473874592e-05</v>
+        <v>-3.687596402640867e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42662696759</v>
+        <v>45699.43227958334</v>
       </c>
     </row>
     <row r="5">
@@ -2211,13 +2211,13 @@
         <v>44202</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.651532411818182e-05</v>
+        <v>-3.986077322560307e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42662696759</v>
+        <v>45699.43227958334</v>
       </c>
     </row>
     <row r="6">
@@ -2228,13 +2228,13 @@
         <v>44258</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.679532411818182e-05</v>
+        <v>-4.014077322560307e-05</v>
       </c>
       <c r="D6" t="n">
         <v>-5e-09</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42662719907</v>
+        <v>45699.43227981481</v>
       </c>
     </row>
     <row r="7">
@@ -2245,13 +2245,13 @@
         <v>44545</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.823032411818182e-05</v>
+        <v>-4.157577322560307e-05</v>
       </c>
       <c r="D7" t="n">
         <v>-5e-09</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45693.42662719907</v>
+        <v>45699.43227981481</v>
       </c>
     </row>
   </sheetData>
@@ -2309,7 +2309,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42676871528</v>
+        <v>45699.4323562963</v>
       </c>
     </row>
     <row r="3">
@@ -2326,7 +2326,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42676886574</v>
+        <v>45699.43235642361</v>
       </c>
     </row>
     <row r="4">
@@ -2343,7 +2343,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42676871528</v>
+        <v>45699.4323562963</v>
       </c>
     </row>
     <row r="5">
@@ -2360,7 +2360,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42676871528</v>
+        <v>45699.4323562963</v>
       </c>
     </row>
   </sheetData>
@@ -2418,7 +2418,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42689134259</v>
+        <v>45699.43242716435</v>
       </c>
     </row>
     <row r="3">
@@ -2435,7 +2435,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42689134259</v>
+        <v>45699.43242716435</v>
       </c>
     </row>
     <row r="4">
@@ -2452,7 +2452,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42689134259</v>
+        <v>45699.43242716435</v>
       </c>
     </row>
     <row r="5">
@@ -2469,7 +2469,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42689134259</v>
+        <v>45699.43242716435</v>
       </c>
     </row>
     <row r="6">
@@ -2486,7 +2486,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42689134259</v>
+        <v>45699.43242716435</v>
       </c>
     </row>
     <row r="7">
@@ -2503,7 +2503,7 @@
         <v>-3e-08</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45693.42689134259</v>
+        <v>45699.43242716435</v>
       </c>
     </row>
   </sheetData>
@@ -2555,13 +2555,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.66114419540266e-05</v>
+        <v>-1.751724226878591e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42216070602</v>
+        <v>45699.42933704861</v>
       </c>
     </row>
     <row r="3">
@@ -2572,13 +2572,13 @@
         <v>41640</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.284468391658289e-05</v>
+        <v>-1.393040611681313e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42216070602</v>
+        <v>45699.42933704861</v>
       </c>
     </row>
     <row r="4">
@@ -2589,13 +2589,13 @@
         <v>42707.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.497968391658289e-05</v>
+        <v>-1.606540611681313e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42216094907</v>
+        <v>45699.42933716435</v>
       </c>
     </row>
     <row r="5">
@@ -2606,13 +2606,13 @@
         <v>43026</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.478880083760723e-05</v>
+        <v>-1.615628266504805e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42216070602</v>
+        <v>45699.42933704861</v>
       </c>
     </row>
     <row r="6">
@@ -2623,13 +2623,13 @@
         <v>44128.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.446163035416667e-05</v>
+        <v>-1.583021587928638e-05</v>
       </c>
       <c r="D6" t="n">
         <v>-2e-09</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42216070602</v>
+        <v>45699.42933704861</v>
       </c>
     </row>
   </sheetData>
@@ -2681,13 +2681,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-8.009535260742326e-06</v>
+        <v>-1.094509649985323e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-1.32e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42243967592</v>
+        <v>45699.42953510417</v>
       </c>
     </row>
     <row r="3">
@@ -2698,13 +2698,13 @@
         <v>41941</v>
       </c>
       <c r="C3" t="n">
-        <v>-9.212055260742326e-06</v>
+        <v>-1.214761649985323e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-1.32e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42243998843</v>
+        <v>45699.42953517361</v>
       </c>
     </row>
     <row r="4">
@@ -2715,13 +2715,13 @@
         <v>42987.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.059343526074233e-05</v>
+        <v>-1.352899649985323e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-1.32e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42243998843</v>
+        <v>45699.42953517361</v>
       </c>
     </row>
     <row r="5">
@@ -2732,13 +2732,13 @@
         <v>43355</v>
       </c>
       <c r="C5" t="n">
-        <v>-8.764960811715929e-06</v>
+        <v>-1.21162281181069e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-1.32e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42243967592</v>
+        <v>45699.42953510417</v>
       </c>
     </row>
     <row r="6">
@@ -2749,13 +2749,13 @@
         <v>44163.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.079476700873556e-06</v>
+        <v>-1.015125986149797e-05</v>
       </c>
       <c r="D6" t="n">
         <v>-1.32e-09</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42243967592</v>
+        <v>45699.42953510417</v>
       </c>
     </row>
   </sheetData>
@@ -2807,13 +2807,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.208654861614519e-05</v>
+        <v>-1.451039239217842e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-4.76e-10</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42263416667</v>
+        <v>45699.42976238426</v>
       </c>
     </row>
     <row r="3">
@@ -2824,13 +2824,13 @@
         <v>41794</v>
       </c>
       <c r="C3" t="n">
-        <v>-8.797444772336551e-06</v>
+        <v>-1.084106635606613e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-4.76e-10</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42263416667</v>
+        <v>45699.42976238426</v>
       </c>
     </row>
     <row r="4">
@@ -2841,13 +2841,13 @@
         <v>42795</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.273920772336551e-06</v>
+        <v>-1.131754235606613e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-4.76e-10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42263444445</v>
+        <v>45699.4297631713</v>
       </c>
     </row>
     <row r="5">
@@ -2858,13 +2858,13 @@
         <v>44079.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-8.864256280629331e-06</v>
+        <v>-1.072990306400241e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-4.76e-10</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42263416667</v>
+        <v>45699.42976238426</v>
       </c>
     </row>
     <row r="6">
@@ -2875,13 +2875,13 @@
         <v>44975.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-8.26026077587623e-06</v>
+        <v>-1.051201808636742e-05</v>
       </c>
       <c r="D6" t="n">
         <v>-4.76e-10</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42263416667</v>
+        <v>45699.42976238426</v>
       </c>
     </row>
   </sheetData>
@@ -2933,13 +2933,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.568106527749864e-05</v>
+        <v>-1.517831388139519e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-8.12e-10</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42288696759</v>
+        <v>45699.43000055556</v>
       </c>
     </row>
     <row r="3">
@@ -2950,13 +2950,13 @@
         <v>42301.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.671352327749864e-05</v>
+        <v>-1.621077188139519e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-8.12e-10</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42288716435</v>
+        <v>45699.43000067129</v>
       </c>
     </row>
     <row r="4">
@@ -2967,13 +2967,13 @@
         <v>43386.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.759454327749864e-05</v>
+        <v>-1.709179188139519e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-8.12e-10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42288716435</v>
+        <v>45699.43000067129</v>
       </c>
     </row>
     <row r="5">
@@ -2984,13 +2984,13 @@
         <v>43750.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.576013026415463e-05</v>
+        <v>-1.518043171774478e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-8.12e-10</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42288696759</v>
+        <v>45699.43000055556</v>
       </c>
     </row>
     <row r="6">
@@ -3001,13 +3001,13 @@
         <v>44954.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-8.82435553633218e-06</v>
+        <v>-8.302379699520973e-06</v>
       </c>
       <c r="D6" t="n">
         <v>-8.12e-10</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42288696759</v>
+        <v>45699.43000055556</v>
       </c>
     </row>
   </sheetData>
@@ -3059,13 +3059,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.736512120756952e-05</v>
+        <v>-1.759504368615993e-05</v>
       </c>
       <c r="D2" t="n">
         <v>-1.5e-09</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42318304398</v>
+        <v>45699.43024622685</v>
       </c>
     </row>
     <row r="3">
@@ -3076,13 +3076,13 @@
         <v>42249</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.919362120756952e-05</v>
+        <v>-1.942354368615993e-05</v>
       </c>
       <c r="D3" t="n">
         <v>-1.5e-09</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42318326389</v>
+        <v>45699.43024650463</v>
       </c>
     </row>
     <row r="4">
@@ -3093,13 +3093,13 @@
         <v>43040</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.93459375261922e-05</v>
+        <v>-1.973271155775566e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-1.5e-09</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42318304398</v>
+        <v>45699.43024622685</v>
       </c>
     </row>
     <row r="5">
@@ -3110,13 +3110,13 @@
         <v>44499.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.004433763426037e-05</v>
+        <v>-2.042309272475929e-05</v>
       </c>
       <c r="D5" t="n">
         <v>-1.5e-09</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42318304398</v>
+        <v>45699.43024622685</v>
       </c>
     </row>
     <row r="6">
@@ -3127,13 +3127,13 @@
         <v>45178.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.106283763426037e-05</v>
+        <v>-2.144159272475929e-05</v>
       </c>
       <c r="D6" t="n">
         <v>-1.5e-09</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42318326389</v>
+        <v>45699.43024650463</v>
       </c>
     </row>
   </sheetData>
@@ -3185,13 +3185,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-9.589542806634301e-06</v>
+        <v>-7.435582698831268e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-4.7e-10</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42329850695</v>
+        <v>45699.43037119213</v>
       </c>
     </row>
     <row r="3">
@@ -3202,13 +3202,13 @@
         <v>44237</v>
       </c>
       <c r="C3" t="n">
-        <v>-9.617430830151785e-06</v>
+        <v>-7.2120271633091e-06</v>
       </c>
       <c r="D3" t="n">
         <v>-4.7e-10</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42329850695</v>
+        <v>45699.43037119213</v>
       </c>
     </row>
     <row r="4">
@@ -3219,13 +3219,13 @@
         <v>45203</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.812269772089445e-06</v>
+        <v>-7.502093079143848e-06</v>
       </c>
       <c r="D4" t="n">
         <v>-4.7e-10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42329850695</v>
+        <v>45699.43037119213</v>
       </c>
     </row>
   </sheetData>
@@ -3277,13 +3277,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.290816691273146e-05</v>
+        <v>-9.14605725073916e-06</v>
       </c>
       <c r="D2" t="n">
         <v>-7.7e-10</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.42352934027</v>
+        <v>45699.43061270833</v>
       </c>
     </row>
     <row r="3">
@@ -3294,13 +3294,13 @@
         <v>41367</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.251746553466974e-05</v>
+        <v>-9.405547250739161e-06</v>
       </c>
       <c r="D3" t="n">
         <v>-7.7e-10</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.42352934027</v>
+        <v>45699.43061288194</v>
       </c>
     </row>
     <row r="4">
@@ -3311,13 +3311,13 @@
         <v>42655</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.189272787390153e-05</v>
+        <v>-8.683072879613658e-06</v>
       </c>
       <c r="D4" t="n">
         <v>-7.7e-10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.42352934027</v>
+        <v>45699.43061270833</v>
       </c>
     </row>
     <row r="5">
@@ -3328,13 +3328,13 @@
         <v>43407.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.247215287390153e-05</v>
+        <v>-9.262497879613658e-06</v>
       </c>
       <c r="D5" t="n">
         <v>-7.7e-10</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.42352965278</v>
+        <v>45699.43061288194</v>
       </c>
     </row>
     <row r="6">
@@ -3345,13 +3345,13 @@
         <v>43771.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.180429018083143e-05</v>
+        <v>-8.270735287072315e-06</v>
       </c>
       <c r="D6" t="n">
         <v>-7.7e-10</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.42352934027</v>
+        <v>45699.43061270833</v>
       </c>
     </row>
     <row r="7">
@@ -3362,13 +3362,13 @@
         <v>44541.5</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.098499137406224e-05</v>
+        <v>-7.903876011465148e-06</v>
       </c>
       <c r="D7" t="n">
         <v>-7.7e-10</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45693.42352934027</v>
+        <v>45699.43061270833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>